<commit_message>
FCM New Test case and Add Vendor and Edit Plan Test Pages and Cases - Changes are done
</commit_message>
<xml_diff>
--- a/Exceldata/User_Information_Automation.xlsx
+++ b/Exceldata/User_Information_Automation.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16425" windowHeight="5970" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="User_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateVendor" sheetId="6" r:id="rId1"/>
+    <sheet name="CreatePlan" sheetId="2" r:id="rId2"/>
+    <sheet name="EditPlan" sheetId="3" r:id="rId3"/>
+    <sheet name="ADDFCM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:N17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>Create Vendor Field Name</t>
   </si>
@@ -55,21 +58,6 @@
     <t>Vendor Mode</t>
   </si>
   <si>
-    <t>LITE/PREMIERE/MOOC</t>
-  </si>
-  <si>
-    <t>PREMIERE</t>
-  </si>
-  <si>
-    <t>PRODUCER/DISTRIBUTOR</t>
-  </si>
-  <si>
-    <t>DISTRIBUTOR</t>
-  </si>
-  <si>
-    <t>Vendor Type</t>
-  </si>
-  <si>
     <t>Plan Interval</t>
   </si>
   <si>
@@ -149,13 +137,154 @@
   </si>
   <si>
     <t>Jeethu@test.com</t>
+  </si>
+  <si>
+    <t>Create Plan Field Name</t>
+  </si>
+  <si>
+    <t>PlanName</t>
+  </si>
+  <si>
+    <t>JeethuPlan</t>
+  </si>
+  <si>
+    <t>PlanType</t>
+  </si>
+  <si>
+    <t>LITE</t>
+  </si>
+  <si>
+    <t>LITE/PREMIERE</t>
+  </si>
+  <si>
+    <t>EnterMonthlyPrice</t>
+  </si>
+  <si>
+    <t>EnterMonthly-Discounted-Price</t>
+  </si>
+  <si>
+    <t>EnterYearlylyPrice</t>
+  </si>
+  <si>
+    <t>EnterYearly-Discounted-Price</t>
+  </si>
+  <si>
+    <t>Vendor-Total-Content-Duration [ in MIN ]</t>
+  </si>
+  <si>
+    <t>Monthly-Watch-Min [ in MIN ]</t>
+  </si>
+  <si>
+    <t>2 Hour</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
+  </si>
+  <si>
+    <t>LiveChannel</t>
+  </si>
+  <si>
+    <t>64 Max Count</t>
+  </si>
+  <si>
+    <t>TrailPeriod</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test Discription</t>
+  </si>
+  <si>
+    <t>Edited - JeethuPlan</t>
+  </si>
+  <si>
+    <t>4 Hour</t>
+  </si>
+  <si>
+    <t>Edited - Test Discription</t>
+  </si>
+  <si>
+    <t>FCM Field Name</t>
+  </si>
+  <si>
+    <t>Enter the Value for the FCM Field</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Premiering Enabled</t>
+  </si>
+  <si>
+    <t>LITE/PREMIERE/MOOC/UGC</t>
+  </si>
+  <si>
+    <t>Subscription Enabled</t>
+  </si>
+  <si>
+    <t>Events Enabled</t>
+  </si>
+  <si>
+    <t>Expiry Enabled</t>
+  </si>
+  <si>
+    <t>Content Expiry (in Days)</t>
+  </si>
+  <si>
+    <t>Rewards Enabled</t>
+  </si>
+  <si>
+    <t>FCM Credentials</t>
+  </si>
+  <si>
+    <t>Stripe Credentials</t>
+  </si>
+  <si>
+    <t>Fortumo Credentials</t>
+  </si>
+  <si>
+    <t>PayPal Credentials</t>
+  </si>
+  <si>
+    <t>PayTM Credentials</t>
+  </si>
+  <si>
+    <t>Braintree Credentials</t>
+  </si>
+  <si>
+    <t>Inapp Credentials</t>
+  </si>
+  <si>
+    <t>FireTV Credentials</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,16 +315,29 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -203,19 +345,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -498,238 +661,674 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>32</v>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="9">
+        <v>7</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B13" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3">
+        <v>99</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3">
+        <v>999</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3">
+        <v>120</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3">
+        <v>99</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3">
+        <v>999</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3">
+        <v>998</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3">
+        <v>120</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3">
+        <v>240</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New FCM and Create Vendor Page Updated
</commit_message>
<xml_diff>
--- a/Exceldata/User_Information_Automation.xlsx
+++ b/Exceldata/User_Information_Automation.xlsx
@@ -13,7 +13,7 @@
     <sheet name="ADDFCM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N17"/>
+  <oleSize ref="A1:C17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>Create Vendor Field Name</t>
   </si>
@@ -278,13 +278,37 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>{"fcmdburl":"","fcmapikey":"","configfile":"","fcmnotifykey":"","fcmuserid":"","projectid":"","authdomain":"","senderid":"","vendorid":""}</t>
+  </si>
+  <si>
+    <t>{"paypalenv" : "" , "paypal_fallbackamount" : "" , "paypal_fallbackcurrency"  : "", "clientid" : "", "secretkey" : ""}</t>
+  </si>
+  <si>
+    <t>{"sandboxmode" : "","merchantid" : "","merchantkey":"","industrytypeid" : "","website" : ""}</t>
+  </si>
+  <si>
+    <t>{"braintreeenv":"" ,"braintreepaypalaccesstoken": "","merchantAccountId": "","braintree_paypal_fallbackamount":"","braintree_paypal_fallbackcurrency": ""}</t>
+  </si>
+  <si>
+    <t>{"sandboxmode" : "","sharedpassword" : "","bundleid" : ""}</t>
+  </si>
+  <si>
+    <t>Demo data</t>
+  </si>
+  <si>
+    <t>Demo Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 - 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +346,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -337,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -360,25 +401,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -663,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,120 +734,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -796,54 +857,54 @@
       <c r="A13" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -851,96 +912,98 @@
       <c r="A18" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>7</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -970,7 +1033,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,120 +1044,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>100</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>99</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>1000</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>999</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>60</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>120</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>1</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1106,7 +1171,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,120 +1182,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="12" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>99</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>98</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>999</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>998</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>120</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>240</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>50</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1242,87 +1309,108 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="145.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C1" s="11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>62</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="9" t="s">
         <v>64</v>
       </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="9" t="s">
         <v>65</v>
       </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>66</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
         <v>63</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="9" t="s">
         <v>68</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="9" t="s">
         <v>84</v>
       </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>